<commit_message>
Fixed issue with result file
</commit_message>
<xml_diff>
--- a/Purchase requests result.xlsx
+++ b/Purchase requests result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\PWC-Purchases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59C2CE1-52EC-4200-BE4C-7FB11F0687A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C153E8DF-FDF0-4FC8-932B-AB8FA5498646}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9218" xr2:uid="{CC834EF1-42AA-4737-8420-7857FAEAC985}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Название компании</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Да</t>
-  </si>
-  <si>
-    <t>http://zakupki.gov.ru/epz/orderplan/extendedsearch/results.html?morphology=on&amp;openMode=USE_DEFAULT_PARAMS&amp;searchType=false&amp;fz44=on&amp;fz223=on&amp;customerTitle=%D0%93%D0%9E%D0%A1%D0%A3%D0%94%D0%90%D0%A0%D0%A1%D0%A2%D0%92%D0%95%D0%9D%D0%9D%D0%9E%D0%95+%D0%91%D0%AE%D0%94%D0%96%D0%95%D0%A2%D0%9D%D0%9E%D0%95+%D0%A3%D0%A7%D0%A0%D0%95%D0%96%D0%94%D0%95%D0%9D%D0%98%D0%95+%D0%97%D0%94%D0%A0%D0%90%D0%92%D0%9E%D0%9E%D0%A5%D0%A0%D0%90%D0%9D%D0%95%D0%9D%D0%98%D0%AF+%D0%A0%D0%95%D0%A1%D0%9F%D0%A3%D0%91%D0%9B%D0%98%D0%9A%D0%98+%D0%90%D0%94%D0%AB%D0%93%D0%95%D0%AF+%22%D0%90%D0%94%D0%AB%D0%93%D0%95%D0%99%D0%A1%D0%9A%D0%90%D0%AF+%D0%A0%D0%95%D0%A1%D0%9F%D0%A3%D0%91%D0%9B%D0%98%D0%9A%D0%90%D0%9D%D0%A1%D0%9A%D0%90%D0%AF+%D0%9A%D0%9B%D0%98%D0%9D%D0%98%D0%A7%D0%95%D0%A1%D0%9A%D0%90%D0%AF+%D0%98%D0%9D%D0%A4%D0%95%D0%9A%D0%A6%D0%98%D0%9E%D0%9D%D0%9D%D0%90%D0%AF+%D0%91%D0%9E%D0%9B%D0%AC%D0%9D%D0%98%D0%A6%D0%90%22&amp;customerCode=03762000148&amp;customerFz94id=1736665&amp;customerFz223id=58171&amp;regionDeleted=false&amp;actualPeriodStart=01.01.2019&amp;actualPeriodEnd=31.12.2019&amp;structured=true&amp;sortBy=BY_MODIFY_DATE&amp;placementRangeMonthFrom=-1&amp;placementRangeMonthTo=-1&amp;currencyId=-1&amp;currencyTotalId=-1&amp;currencySMBId=-1&amp;executionRangeMonthFrom=-1&amp;executionRangeMonthTo=-1&amp;pageNumber=1&amp;sortDirection=false&amp;recordsPerPage=_10</t>
   </si>
   <si>
     <t>http://zakupki.gov.ru/epz/orderplan/extendedsearch/results.html?morphology=on&amp;openMode=USE_DEFAULT_PARAMS&amp;searchType=false&amp;fz44=on&amp;fz223=on&amp;customerTitle=%D0%9C%D0%A3%D0%9D%D0%98%D0%A6%D0%98%D0%9F%D0%90%D0%9B%D0%AC%D0%9D%D0%9E%D0%95+%D0%90%D0%92%D0%A2%D0%9E%D0%9D%D0%9E%D0%9C%D0%9D%D0%9E%D0%95+%D0%9E%D0%91%D0%A9%D0%95%D0%9E%D0%91%D0%A0%D0%90%D0%97%D0%9E%D0%92%D0%90%D0%A2%D0%95%D0%9B%D0%AC%D0%9D%D0%9E%D0%95+%D0%A3%D0%A7%D0%A0%D0%95%D0%96%D0%94%D0%95%D0%9D%D0%98%D0%95+%22%D0%A1%D0%A0%D0%95%D0%94%D0%9D%D0%AF%D0%AF+%D0%9E%D0%91%D0%A9%D0%95%D0%9E%D0%91%D0%A0%D0%90%D0%97%D0%9E%D0%92%D0%90%D0%A2%D0%95%D0%9B%D0%AC%D0%9D%D0%90%D0%AF+%D0%A8%D0%9A%D0%9E%D0%9B%D0%90+%E2%84%96+77+%D0%A1+%D0%A3%D0%93%D0%9B%D0%A3%D0%91%D0%9B%D0%95%D0%9D%D0%9D%D0%AB%D0%9C+%D0%98%D0%97%D0%A3%D0%A7%D0%95%D0%9D%D0%98%D0%95%D0%9C+%D0%90%D0%9D%D0%93%D0%9B%D0%98%D0%99%D0%A1%D0%9A%D0%9E%D0%93%D0%9E+%D0%AF%D0%97%D0%AB%D0%9A%D0%90%22+%D0%93.%D0%9F%D0%95%D0%A0%D0%9C%D0%98&amp;customerCode=03563000083&amp;customerFz94id=785202&amp;customerFz223id=180825&amp;regionDeleted=false&amp;actualPeriodStart=01.01.2019&amp;actualPeriodEnd=31.12.2019&amp;structured=true&amp;sortBy=BY_MODIFY_DATE&amp;placementRangeMonthFrom=-1&amp;placementRangeMonthTo=-1&amp;currencyId=-1&amp;currencyTotalId=-1&amp;currencySMBId=-1&amp;executionRangeMonthFrom=-1&amp;executionRangeMonthTo=-1&amp;pageNumber=1&amp;sortDirection=false&amp;recordsPerPage=_10</t>
@@ -511,17 +508,14 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
+      <c r="A4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
         <v>105020580</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -535,7 +529,7 @@
         <v>5904082422</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
output sheet changed, code refactored
</commit_message>
<xml_diff>
--- a/Purchase requests result.xlsx
+++ b/Purchase requests result.xlsx
@@ -1,38 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\PWC-Purchases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18ACCA-B6AE-4D8F-99C3-B053B4951CC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C36BA79-6C12-4DD3-B695-C47A0EF1B576}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2280" windowWidth="10710" windowHeight="10417" activeTab="1" xr2:uid="{6CCDD2E9-C472-4690-910A-E00ED6FFC8F7}"/>
+    <workbookView xWindow="675" yWindow="2280" windowWidth="10710" windowHeight="10417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Закупки" sheetId="2" r:id="rId2"/>
+    <sheet name="Закупки" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Статус</t>
   </si>
@@ -67,34 +55,17 @@
     <t>7736050003</t>
   </si>
   <si>
-    <t>Да</t>
-  </si>
-  <si>
     <t>ГОСУДАРСТВЕННОЕ БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ РЕСПУБЛИКИ АДЫГЕЯ "АДЫГЕЙСКАЯ РЕСПУБЛИКАНСКАЯ КЛИНИЧЕСКАЯ ИНФЕКЦИОННАЯ БОЛЬНИЦА"</t>
   </si>
   <si>
     <t>105020580</t>
-  </si>
-  <si>
-    <t>http://zakupki.gov.ru/epz/orderplan/extendedsearch/results.html?morphology=on&amp;openMode=USE_DEFAULT_PARAMS&amp;searchType=false&amp;fz44=on&amp;fz223=on&amp;customerTitle=%D0%93%D0%9E%D0%A1%D0%A3%D0%94%D0%90%D0%A0%D0%A1%D0%A2%D0%92%D0%95%D0%9D%D0%9D%D0%9E%D0%95+%D0%91%D0%AE%D0%94%D0%96%D0%95%D0%A2%D0%9D%D0%9E%D0%95+%D0%A3%D0%A7%D0%A0%D0%95%D0%96%D0%94%D0%95%D0%9D%D0%98%D0%95+%D0%97%D0%94%D0%A0%D0%90%D0%92%D0%9E%D0%9E%D0%A5%D0%A0%D0%90%D0%9D%D0%95%D0%9D%D0%98%D0%AF+%D0%A0%D0%95%D0%A1%D0%9F%D0%A3%D0%91%D0%9B%D0%98%D0%9A%D0%98+%D0%90%D0%94%D0%AB%D0%93%D0%95%D0%AF+%22%D0%90%D0%94%D0%AB%D0%93%D0%95%D0%99%D0%A1%D0%9A%D0%90%D0%AF+%D0%A0%D0%95%D0%A1%D0%9F%D0%A3%D0%91%D0%9B%D0%98%D0%9A%D0%90%D0%9D%D0%A1%D0%9A%D0%90%D0%AF+%D0%9A%D0%9B%D0%98%D0%9D%D0%98%D0%A7%D0%95%D0%A1%D0%9A%D0%90%D0%AF+%D0%98%D0%9D%D0%A4%D0%95%D0%9A%D0%A6%D0%98%D0%9E%D0%9D%D0%9D%D0%90%D0%AF+%D0%91%D0%9E%D0%9B%D0%AC%D0%9D%D0%98%D0%A6%D0%90%22&amp;customerCode=03762000148&amp;customerFz94id=1736665&amp;customerFz223id=58171&amp;regionDeleted=false&amp;actualPeriodStart=01.01.2019&amp;actualPeriodEnd=31.12.2019&amp;structured=true&amp;sortBy=BY_MODIFY_DATE&amp;placementRangeMonthFrom=-1&amp;placementRangeMonthTo=-1&amp;currencyId=-1&amp;currencyTotalId=-1&amp;currencySMBId=-1&amp;executionRangeMonthFrom=-1&amp;executionRangeMonthTo=-1&amp;pageNumber=1&amp;sortDirection=false&amp;recordsPerPage=_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +92,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,40 +105,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{39120A7B-7E35-4240-8BA2-D93A9025C0FF}"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -192,11 +148,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -220,24 +176,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E28F431-50DC-4E37-843E-EA25A0ECAA07}" name="Таблица1" displayName="Таблица1" ref="A1:F4" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F4" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F4" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{209245A5-C0D1-4723-88CB-F71A5DF95FEC}" name="Статус" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{EA613A85-2EB4-4996-9E36-46EFB5780FE6}" name="Название компании" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{37B4E908-7428-4621-B85A-D4BE54A74A6E}" name="ИНН" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{ED7E0E0A-806B-4453-A8F9-3310441E551B}" name="Начало периода" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{CB62AD9D-0A35-4C79-9D63-A7369A608587}" name="Окончание периода" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A33FB6E3-F54C-47FD-83DA-3CADE36A4B1E}" name="Ссылка" dataDxfId="2" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="1" xr3:uid="{CFB6E728-64A8-4ADF-BDB3-A1E196E36295}" name="Статус" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8AB05E53-751C-4C31-98E0-0B3AB86B97AF}" name="Название компании" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2D836B73-6073-464E-8A65-45719478164D}" name="ИНН" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{70556501-B593-419F-9AAA-564826304ACB}" name="Начало периода" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B63A20C1-7098-4D7C-AA83-8249B66CCA46}" name="Окончание периода" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4338B633-B471-472B-986F-66F32040775F}" name="Ссылка" dataDxfId="2" dataCellStyle="Гиперссылка"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -251,7 +207,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -263,7 +219,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -275,12 +231,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -310,29 +266,12 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -362,26 +301,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,32 +452,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51FFAFC-3052-4F23-BD6C-49678BD9FF8E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939D229D-AF79-43A5-9FE8-64BD21253489}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702B5DF7-8DAE-4FF5-87DD-7EBCF11EC697}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="30.53125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.06640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.86328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.53125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="5"/>
+    <col min="1" max="1" width="11.06640625" customWidth="1"/>
+    <col min="2" max="2" width="30.53125" customWidth="1"/>
+    <col min="3" max="3" width="23.06640625" customWidth="1"/>
+    <col min="4" max="4" width="16.265625" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" customWidth="1"/>
+    <col min="6" max="6" width="24.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -579,7 +490,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -597,7 +508,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -606,29 +517,27 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="3">
         <v>43116</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>43486</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
high-load bug fixed, specification updated
</commit_message>
<xml_diff>
--- a/Purchase requests result.xlsx
+++ b/Purchase requests result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C36BA79-6C12-4DD3-B695-C47A0EF1B576}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615BF95-11B8-4048-9D3D-F3120DA7F35D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="2280" windowWidth="10710" windowHeight="10417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="16">
   <si>
     <t>Статус</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>105020580</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>"ГАЗПРОМ"</t>
+  </si>
+  <si>
+    <t>http://zakupki.gov.ru/epz/orderplan/extendedsearch/results.html?morphology=on&amp;openMode=USE_DEFAULT_PARAMS&amp;searchType=false&amp;fz44=on&amp;fz223=on&amp;customerTitle=%D0%9F%D0%A3%D0%91%D0%9B%D0%98%D0%A7%D0%9D%D0%9E%D0%95+%D0%90%D0%9A%D0%A6%D0%98%D0%9E%D0%9D%D0%95%D0%A0%D0%9D%D0%9E%D0%95+%D0%9E%D0%91%D0%A9%D0%95%D0%A1%D0%A2%D0%92%D0%9E+%22%D0%93%D0%90%D0%97%D0%9F%D0%A0%D0%9E%D0%9C%22&amp;customerCode=06730000003&amp;customerFz94id=816861&amp;customerFz223id=8849&amp;regionDeleted=false&amp;actualPeriodStart=01.01.2019&amp;actualPeriodEnd=31.12.2019&amp;structured=true&amp;sortBy=BY_MODIFY_DATE&amp;placementRangeMonthFrom=-1&amp;placementRangeMonthTo=-1&amp;currencyId=-1&amp;currencyTotalId=-1&amp;currencySMBId=-1&amp;executionRangeMonthFrom=-1&amp;executionRangeMonthTo=-1&amp;pageNumber=1&amp;sortDirection=false&amp;recordsPerPage=_10</t>
   </si>
 </sst>
 </file>
@@ -82,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -124,6 +139,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -176,8 +194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F4" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F4" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F24" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F24" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CFB6E728-64A8-4ADF-BDB3-A1E196E36295}" name="Статус" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{8AB05E53-751C-4C31-98E0-0B3AB86B97AF}" name="Название компании" dataDxfId="1"/>
@@ -453,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702B5DF7-8DAE-4FF5-87DD-7EBCF11EC697}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -539,6 +557,326 @@
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
+    <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>